<commit_message>
Committing after changing performance excel file
</commit_message>
<xml_diff>
--- a/Tree_Performance/runtime_vs_accuracy_perf.xlsx
+++ b/Tree_Performance/runtime_vs_accuracy_perf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Desktop/NeuralNetworkTree/Tree_Performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042EB122-3B4A-B040-8CA7-7F5FF235B630}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAADF18-EED9-9445-8192-6340C704B662}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="16540" xr2:uid="{F805375B-28AA-40B3-8F64-3973FA971C22}"/>
   </bookViews>
@@ -232,6 +232,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$21</c:f>
@@ -354,6 +408,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$21</c:f>
@@ -430,8 +538,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -470,6 +579,59 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$21</c:f>
@@ -574,6 +736,59 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$21</c:f>
@@ -652,7 +867,7 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -670,6 +885,59 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Run</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -705,6 +973,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="82537743"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -760,6 +1029,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="81858783"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1352,12 +1622,12 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>

</xml_diff>